<commit_message>
Added cmip5 vocab mappings
</commit_message>
<xml_diff>
--- a/mappings/cmip5-ocean.component-tree.xlsx
+++ b/mappings/cmip5-ocean.component-tree.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/esdoc-docs/cmip5/vocab-mappings/ocean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6-specializations-ocean/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27300" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Table 1</t>
   </si>
@@ -105,6 +105,39 @@
   </si>
   <si>
     <t>cmip6-id</t>
+  </si>
+  <si>
+    <t>cmip6.ocean</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.advection</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.boundary_forcing</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.boundary_forcing.tracers</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics.momentum</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics.tracers</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.uplow_boundaries</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics.interior_mixing</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics.boundary_layer_mixing</t>
   </si>
 </sst>
 </file>
@@ -1500,13 +1533,15 @@
   <dimension ref="A1:IV13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="51.6640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="24.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="1" customWidth="1"/>
     <col min="5" max="256" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1539,7 +1574,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="D3" s="7">
         <v>0</v>
       </c>
@@ -1551,7 +1588,9 @@
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="11">
         <v>0</v>
       </c>
@@ -1563,7 +1602,9 @@
       <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -1575,7 +1616,9 @@
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="D6" s="11">
         <v>0</v>
       </c>
@@ -1587,7 +1630,9 @@
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="11">
         <v>0</v>
       </c>
@@ -1599,7 +1644,9 @@
       <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="D8" s="11">
         <v>0</v>
       </c>
@@ -1611,7 +1658,9 @@
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="11">
         <v>0</v>
       </c>
@@ -1623,7 +1672,9 @@
       <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="D10" s="11">
         <v>0</v>
       </c>
@@ -1635,7 +1686,9 @@
       <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="11">
         <v>0</v>
       </c>
@@ -1647,7 +1700,9 @@
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="11">
         <v>0</v>
       </c>
@@ -1659,7 +1714,9 @@
       <c r="B13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="D13" s="11">
         <v>0</v>
       </c>

</xml_diff>